<commit_message>
V1.3.1 edit photo tran
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\condo-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3DF1E-E5F2-40F4-905F-F25F6AF984D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FAC4A3-8BAD-4619-A7F4-9203856B1118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
   <si>
     <t>id</t>
   </si>
@@ -573,6 +573,21 @@
   </si>
   <si>
     <t>照片</t>
+  </si>
+  <si>
+    <t>addPhoto</t>
+  </si>
+  <si>
+    <t>Add Photo</t>
+  </si>
+  <si>
+    <t>เพิ่มรูปภาพ</t>
+  </si>
+  <si>
+    <t>添加照片</t>
+  </si>
+  <si>
+    <t>写真を追加</t>
   </si>
 </sst>
 </file>
@@ -944,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,6 +1579,23 @@
         <v>177</v>
       </c>
     </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" t="s">
+        <v>180</v>
+      </c>
+      <c r="C37" t="s">
+        <v>181</v>
+      </c>
+      <c r="D37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>